<commit_message>
Updated Bug Tracker With Fix
</commit_message>
<xml_diff>
--- a/Tag/TagBugTracker.xlsx
+++ b/Tag/TagBugTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajan Dev\Desktop\Tag Game\TagGame\Tag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56598B42-0AF2-4ED2-97F4-CD0D296B1A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E1AAEC-55B8-4118-93E9-FC559FF51F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Bug ID</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>Use server travel on session destroyed delegate</t>
   </si>
 </sst>
 </file>
@@ -81,7 +84,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -114,7 +117,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -399,7 +402,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,7 +414,7 @@
     <col min="5" max="5" width="37.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" customWidth="1"/>
     <col min="7" max="7" width="24.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -461,6 +464,12 @@
       </c>
       <c r="F3">
         <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45528</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>